<commit_message>
Commit from GitHub Actions (inac_data)
</commit_message>
<xml_diff>
--- a/econuy_extras/retrieval/faena.xlsx
+++ b/econuy_extras/retrieval/faena.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\GIF\VAS\PUBLICACIONES\INFORME SEMANAL FAENA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FC3989-EB5D-43E9-BDF4-2742B2216152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D7487A-7910-4D76-AFB4-EF184ADD99F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-4695" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -677,13 +677,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1055"/>
+  <dimension ref="A1:I1056"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="9" topLeftCell="C1046" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H1055" sqref="H1055"/>
+      <selection pane="bottomRight" activeCell="K1062" sqref="K1062"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28021,6 +28021,33 @@
       <c r="H1055" s="3">
         <f>SUM(C1055:G1055)</f>
         <v>50726</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1056" s="14">
+        <v>45676</v>
+      </c>
+      <c r="B1056" s="14">
+        <v>45682</v>
+      </c>
+      <c r="C1056" s="3">
+        <v>24948</v>
+      </c>
+      <c r="D1056" s="3">
+        <v>19901</v>
+      </c>
+      <c r="E1056" s="3">
+        <v>8515</v>
+      </c>
+      <c r="F1056" s="3">
+        <v>122</v>
+      </c>
+      <c r="G1056" s="3">
+        <v>779</v>
+      </c>
+      <c r="H1056" s="3">
+        <f>SUM(C1056:G1056)</f>
+        <v>54265</v>
       </c>
     </row>
   </sheetData>
@@ -28042,13 +28069,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H1055"/>
+  <dimension ref="A1:H1056"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="9" topLeftCell="C1047" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G1055" sqref="G1055"/>
+      <selection pane="bottomRight" activeCell="J1061" sqref="J1061"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55283,7 +55310,7 @@
         <v>5779</v>
       </c>
       <c r="H1054" s="3">
-        <f t="shared" ref="H1054:H1055" si="15">SUM(C1054:G1054)</f>
+        <f t="shared" ref="H1054:H1056" si="15">SUM(C1054:G1054)</f>
         <v>21512</v>
       </c>
     </row>
@@ -55312,6 +55339,33 @@
       <c r="H1055" s="3">
         <f t="shared" si="15"/>
         <v>13814</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1056" s="14">
+        <v>45676</v>
+      </c>
+      <c r="B1056" s="14">
+        <v>45682</v>
+      </c>
+      <c r="C1056" s="3">
+        <v>1765</v>
+      </c>
+      <c r="D1056" s="3">
+        <v>1515</v>
+      </c>
+      <c r="E1056">
+        <v>78</v>
+      </c>
+      <c r="F1056" s="3">
+        <v>5057</v>
+      </c>
+      <c r="G1056" s="3">
+        <v>7184</v>
+      </c>
+      <c r="H1056" s="3">
+        <f t="shared" si="15"/>
+        <v>15599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>